<commit_message>
Update test results data - 2025-03-12 11:30 PM
Generated with VH Results Processing System

Processing completed:

- Processed IBA tests (Simple and Full)

- Processed FBS mock tests

- Generated optimized JSON files for Vercel deployment

- Updated students database

- Synced student emails from MongoDB

- Synced roleNumbers to MongoDB for FBS access
</commit_message>
<xml_diff>
--- a/Results/DU FBS Mocks/DU FBS Mock 5.xlsx
+++ b/Results/DU FBS Mocks/DU FBS Mock 5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\results giver\FBS Result Giver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCD92486-F058-4B68-BD30-A70503E0BEE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE50521-A704-44D1-BC2E-2B3DC79D9D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1346" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1382" uniqueCount="189">
   <si>
     <t>ID</t>
   </si>
@@ -352,222 +352,222 @@
     <t>q22</t>
   </si>
   <si>
+    <t>q24</t>
+  </si>
+  <si>
+    <t>q27</t>
+  </si>
+  <si>
+    <t>q36</t>
+  </si>
+  <si>
+    <t>q33</t>
+  </si>
+  <si>
+    <t>q32</t>
+  </si>
+  <si>
+    <t>q48</t>
+  </si>
+  <si>
+    <t>q51</t>
+  </si>
+  <si>
+    <t>q59</t>
+  </si>
+  <si>
+    <t>q61</t>
+  </si>
+  <si>
+    <t>q66</t>
+  </si>
+  <si>
+    <t>q74</t>
+  </si>
+  <si>
+    <t>q12</t>
+  </si>
+  <si>
+    <t>q16</t>
+  </si>
+  <si>
+    <t>q17</t>
+  </si>
+  <si>
+    <t>q25</t>
+  </si>
+  <si>
+    <t>q41</t>
+  </si>
+  <si>
+    <t>q40</t>
+  </si>
+  <si>
+    <t>q38</t>
+  </si>
+  <si>
+    <t>q55</t>
+  </si>
+  <si>
+    <t>q60</t>
+  </si>
+  <si>
+    <t>q45</t>
+  </si>
+  <si>
+    <t>q63</t>
+  </si>
+  <si>
+    <t>q71</t>
+  </si>
+  <si>
+    <t>q75</t>
+  </si>
+  <si>
+    <t>q13</t>
+  </si>
+  <si>
+    <t>q11</t>
+  </si>
+  <si>
+    <t>q10</t>
+  </si>
+  <si>
+    <t>q19</t>
+  </si>
+  <si>
     <t>q28</t>
   </si>
   <si>
-    <t>q27</t>
-  </si>
-  <si>
-    <t>q36</t>
-  </si>
-  <si>
-    <t>q33</t>
-  </si>
-  <si>
-    <t>q32</t>
-  </si>
-  <si>
-    <t>q48</t>
-  </si>
-  <si>
-    <t>q59</t>
-  </si>
-  <si>
-    <t>q45</t>
-  </si>
-  <si>
-    <t>q61</t>
-  </si>
-  <si>
-    <t>q75</t>
-  </si>
-  <si>
-    <t>q74</t>
-  </si>
-  <si>
-    <t>q12</t>
-  </si>
-  <si>
-    <t>q16</t>
-  </si>
-  <si>
-    <t>q17</t>
-  </si>
-  <si>
-    <t>q24</t>
-  </si>
-  <si>
-    <t>q25</t>
-  </si>
-  <si>
     <t>q34</t>
   </si>
   <si>
-    <t>q40</t>
-  </si>
-  <si>
-    <t>q38</t>
-  </si>
-  <si>
-    <t>q55</t>
-  </si>
-  <si>
-    <t>q51</t>
+    <t>q35</t>
+  </si>
+  <si>
+    <t>q56</t>
+  </si>
+  <si>
+    <t>q46</t>
   </si>
   <si>
     <t>q47</t>
   </si>
   <si>
-    <t>q63</t>
-  </si>
-  <si>
-    <t>q71</t>
-  </si>
-  <si>
-    <t>q13</t>
-  </si>
-  <si>
-    <t>q11</t>
-  </si>
-  <si>
-    <t>q10</t>
-  </si>
-  <si>
-    <t>q19</t>
-  </si>
-  <si>
-    <t>q41</t>
+    <t>q70</t>
+  </si>
+  <si>
+    <t>q2</t>
+  </si>
+  <si>
+    <t>q7</t>
+  </si>
+  <si>
+    <t>q6</t>
+  </si>
+  <si>
+    <t>q20</t>
+  </si>
+  <si>
+    <t>q18</t>
+  </si>
+  <si>
+    <t>q23</t>
+  </si>
+  <si>
+    <t>q29</t>
+  </si>
+  <si>
+    <t>q44</t>
+  </si>
+  <si>
+    <t>q42</t>
+  </si>
+  <si>
+    <t>q50</t>
+  </si>
+  <si>
+    <t>q49</t>
+  </si>
+  <si>
+    <t>q73</t>
+  </si>
+  <si>
+    <t>q72</t>
+  </si>
+  <si>
+    <t>q67</t>
+  </si>
+  <si>
+    <t>q3</t>
+  </si>
+  <si>
+    <t>q21</t>
+  </si>
+  <si>
+    <t>q26</t>
+  </si>
+  <si>
+    <t>q30</t>
+  </si>
+  <si>
+    <t>q39</t>
+  </si>
+  <si>
+    <t>q54</t>
+  </si>
+  <si>
+    <t>q58</t>
+  </si>
+  <si>
+    <t>q52</t>
+  </si>
+  <si>
+    <t>q76</t>
+  </si>
+  <si>
+    <t>q65</t>
+  </si>
+  <si>
+    <t>q69</t>
+  </si>
+  <si>
+    <t>q4</t>
+  </si>
+  <si>
+    <t>q8</t>
   </si>
   <si>
     <t>q43</t>
   </si>
   <si>
-    <t>q35</t>
-  </si>
-  <si>
-    <t>q56</t>
+    <t>q53</t>
+  </si>
+  <si>
+    <t>q62</t>
+  </si>
+  <si>
+    <t>q5</t>
+  </si>
+  <si>
+    <t>q31</t>
   </si>
   <si>
     <t>q57</t>
   </si>
   <si>
-    <t>q49</t>
-  </si>
-  <si>
-    <t>q70</t>
-  </si>
-  <si>
-    <t>q66</t>
-  </si>
-  <si>
-    <t>q2</t>
-  </si>
-  <si>
-    <t>q7</t>
-  </si>
-  <si>
-    <t>q6</t>
-  </si>
-  <si>
-    <t>q20</t>
-  </si>
-  <si>
-    <t>q18</t>
-  </si>
-  <si>
-    <t>q23</t>
-  </si>
-  <si>
-    <t>q29</t>
-  </si>
-  <si>
-    <t>q44</t>
-  </si>
-  <si>
-    <t>q42</t>
-  </si>
-  <si>
-    <t>q46</t>
-  </si>
-  <si>
-    <t>q60</t>
-  </si>
-  <si>
-    <t>q52</t>
-  </si>
-  <si>
-    <t>q76</t>
-  </si>
-  <si>
-    <t>q72</t>
-  </si>
-  <si>
-    <t>q67</t>
-  </si>
-  <si>
-    <t>q3</t>
-  </si>
-  <si>
-    <t>q21</t>
-  </si>
-  <si>
-    <t>q26</t>
-  </si>
-  <si>
-    <t>q30</t>
-  </si>
-  <si>
-    <t>q54</t>
-  </si>
-  <si>
-    <t>q53</t>
-  </si>
-  <si>
     <t>q64</t>
   </si>
   <si>
-    <t>q73</t>
-  </si>
-  <si>
-    <t>q62</t>
-  </si>
-  <si>
-    <t>q4</t>
-  </si>
-  <si>
-    <t>q8</t>
-  </si>
-  <si>
-    <t>q31</t>
-  </si>
-  <si>
-    <t>q39</t>
-  </si>
-  <si>
-    <t>q50</t>
-  </si>
-  <si>
-    <t>q58</t>
-  </si>
-  <si>
-    <t>q65</t>
-  </si>
-  <si>
-    <t>q69</t>
-  </si>
-  <si>
-    <t>q5</t>
+    <t>q68</t>
+  </si>
+  <si>
+    <t>q9</t>
   </si>
   <si>
     <t>q37</t>
   </si>
   <si>
-    <t>q68</t>
-  </si>
-  <si>
-    <t>q9</t>
-  </si>
-  <si>
     <t>Roll</t>
   </si>
   <si>
@@ -602,9 +602,6 @@
   </si>
   <si>
     <t>CD (W)</t>
-  </si>
-  <si>
-    <t>BD (W)</t>
   </si>
 </sst>
 </file>
@@ -1254,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI27"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="79" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="AE14" sqref="AE14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1386,18 +1383,18 @@
         <v>92.1875</v>
       </c>
       <c r="G2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H2">
         <v>4</v>
       </c>
       <c r="I2">
         <f t="shared" ref="I2:I26" si="2">G2*1 + H2*($AI$8)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J2">
         <f t="shared" ref="J2:J26" si="3">I2/$AH$2*100</f>
-        <v>50</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="K2">
         <v>0</v>
@@ -1417,41 +1414,41 @@
         <v>8</v>
       </c>
       <c r="P2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="Q2">
         <f t="shared" ref="Q2:Q26" si="6">O2*1 + P2*($AI$8)</f>
-        <v>6.25</v>
+        <v>6</v>
       </c>
       <c r="R2">
         <f t="shared" ref="R2:R26" si="7">Q2/$AH$4*100</f>
-        <v>39.0625</v>
+        <v>37.5</v>
       </c>
       <c r="S2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="T2">
         <v>0</v>
       </c>
       <c r="U2">
         <f t="shared" ref="U2:U26" si="8">S2*1 + T2*($AI$8)</f>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="V2">
         <f t="shared" ref="V2:V26" si="9">U2/$AH$5*100</f>
-        <v>93.75</v>
+        <v>100</v>
       </c>
       <c r="W2">
         <f t="shared" ref="W2:W26" si="10">E2 + I2 + M2 +Q2+U2</f>
-        <v>42</v>
+        <v>43.75</v>
       </c>
       <c r="X2">
         <f t="shared" ref="X2:X26" si="11">W2/($AH$6-16)*100</f>
-        <v>70</v>
+        <v>72.916666666666657</v>
       </c>
       <c r="Y2">
         <f t="shared" ref="Y2:Y26" si="12">_xlfn.RANK.EQ(X2, $X$2:$X$1002, 0)</f>
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="Z2" s="19">
         <v>3</v>
@@ -1468,7 +1465,7 @@
       </c>
       <c r="AE2">
         <f t="shared" ref="AE2:AE26" si="13">W2+Z2+AA2+AB2+AD2+AC2</f>
-        <v>63</v>
+        <v>64.75</v>
       </c>
       <c r="AF2">
         <f t="shared" ref="AF2:AF26" si="14">_xlfn.RANK.EQ(AE2, $AE$2:$AE$1002, 0)</f>
@@ -1501,18 +1498,18 @@
         <v>84.375</v>
       </c>
       <c r="G3">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3">
         <f t="shared" si="2"/>
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
       <c r="J3">
         <f t="shared" si="3"/>
-        <v>70.833333333333343</v>
+        <v>79.166666666666657</v>
       </c>
       <c r="K3">
         <v>10</v>
@@ -1543,26 +1540,26 @@
         <v>0</v>
       </c>
       <c r="S3">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="T3">
         <v>3</v>
       </c>
       <c r="U3">
         <f t="shared" si="8"/>
-        <v>10.25</v>
+        <v>11.25</v>
       </c>
       <c r="V3">
         <f t="shared" si="9"/>
-        <v>64.0625</v>
+        <v>70.3125</v>
       </c>
       <c r="W3">
         <f t="shared" si="10"/>
-        <v>41.25</v>
+        <v>43.25</v>
       </c>
       <c r="X3">
         <f t="shared" si="11"/>
-        <v>68.75</v>
+        <v>72.083333333333329</v>
       </c>
       <c r="Y3">
         <f t="shared" si="12"/>
@@ -1583,11 +1580,11 @@
       </c>
       <c r="AE3">
         <f t="shared" si="13"/>
-        <v>66.25</v>
+        <v>68.25</v>
       </c>
       <c r="AF3">
         <f t="shared" si="14"/>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="AG3" s="13"/>
       <c r="AH3">
@@ -1630,18 +1627,18 @@
         <v>79.166666666666657</v>
       </c>
       <c r="K4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="L4">
         <v>7</v>
       </c>
       <c r="M4">
         <f t="shared" si="4"/>
-        <v>6.25</v>
+        <v>7.25</v>
       </c>
       <c r="N4">
         <f t="shared" si="5"/>
-        <v>39.0625</v>
+        <v>45.3125</v>
       </c>
       <c r="O4">
         <v>0</v>
@@ -1673,15 +1670,15 @@
       </c>
       <c r="W4">
         <f t="shared" si="10"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="X4">
         <f t="shared" si="11"/>
-        <v>71.666666666666671</v>
+        <v>73.333333333333329</v>
       </c>
       <c r="Y4">
         <f t="shared" si="12"/>
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="Z4" s="22">
         <v>3</v>
@@ -1698,7 +1695,7 @@
       </c>
       <c r="AE4">
         <f t="shared" si="13"/>
-        <v>69.5</v>
+        <v>70.5</v>
       </c>
       <c r="AF4">
         <f t="shared" si="14"/>
@@ -1796,7 +1793,7 @@
       </c>
       <c r="Y5">
         <f t="shared" si="12"/>
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="Z5" s="20">
         <v>5.5</v>
@@ -1817,7 +1814,7 @@
       </c>
       <c r="AF5">
         <f t="shared" si="14"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AG5" s="13"/>
       <c r="AH5">
@@ -1911,7 +1908,7 @@
       </c>
       <c r="Y6">
         <f t="shared" si="12"/>
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="Z6" s="20">
         <v>6.5</v>
@@ -2065,41 +2062,41 @@
         <v>4</v>
       </c>
       <c r="P8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="Q8">
         <f t="shared" si="6"/>
-        <v>2.25</v>
+        <v>1.75</v>
       </c>
       <c r="R8">
         <f t="shared" si="7"/>
-        <v>14.0625</v>
+        <v>10.9375</v>
       </c>
       <c r="S8">
         <v>12</v>
       </c>
       <c r="T8">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="U8">
         <f t="shared" si="8"/>
-        <v>11.25</v>
+        <v>11</v>
       </c>
       <c r="V8">
         <f t="shared" si="9"/>
-        <v>70.3125</v>
+        <v>68.75</v>
       </c>
       <c r="W8">
         <f t="shared" si="10"/>
-        <v>39</v>
+        <v>38.25</v>
       </c>
       <c r="X8">
         <f t="shared" si="11"/>
-        <v>65</v>
+        <v>63.749999999999993</v>
       </c>
       <c r="Y8">
         <f t="shared" si="12"/>
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="Z8" s="19">
         <v>6.5</v>
@@ -2116,7 +2113,7 @@
       </c>
       <c r="AE8">
         <f t="shared" si="13"/>
-        <v>58.5</v>
+        <v>57.75</v>
       </c>
       <c r="AF8">
         <f t="shared" si="14"/>
@@ -2162,32 +2159,32 @@
         <v>50</v>
       </c>
       <c r="K9">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="L9">
         <v>3</v>
       </c>
       <c r="M9">
         <f t="shared" si="4"/>
-        <v>7.25</v>
+        <v>9.25</v>
       </c>
       <c r="N9">
         <f t="shared" si="5"/>
-        <v>45.3125</v>
+        <v>57.8125</v>
       </c>
       <c r="O9">
         <v>4</v>
       </c>
       <c r="P9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="Q9">
         <f t="shared" si="6"/>
-        <v>2.5</v>
+        <v>2</v>
       </c>
       <c r="R9">
         <f t="shared" si="7"/>
-        <v>15.625</v>
+        <v>12.5</v>
       </c>
       <c r="S9">
         <v>0</v>
@@ -2205,11 +2202,11 @@
       </c>
       <c r="W9">
         <f t="shared" si="10"/>
-        <v>27</v>
+        <v>28.5</v>
       </c>
       <c r="X9">
         <f t="shared" si="11"/>
-        <v>45</v>
+        <v>47.5</v>
       </c>
       <c r="Y9">
         <f t="shared" si="12"/>
@@ -2230,7 +2227,7 @@
       <c r="AD9" s="21"/>
       <c r="AE9">
         <f t="shared" si="13"/>
-        <v>41</v>
+        <v>42.5</v>
       </c>
       <c r="AF9">
         <f t="shared" si="14"/>
@@ -2349,15 +2346,15 @@
         <v>5</v>
       </c>
       <c r="L11">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M11">
         <f t="shared" si="4"/>
-        <v>2.5</v>
+        <v>2.25</v>
       </c>
       <c r="N11">
         <f t="shared" si="5"/>
-        <v>15.625</v>
+        <v>14.0625</v>
       </c>
       <c r="O11">
         <v>0</v>
@@ -2377,27 +2374,27 @@
         <v>14</v>
       </c>
       <c r="T11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U11">
         <f t="shared" si="8"/>
-        <v>13.75</v>
+        <v>13.5</v>
       </c>
       <c r="V11">
         <f t="shared" si="9"/>
-        <v>85.9375</v>
+        <v>84.375</v>
       </c>
       <c r="W11">
         <f t="shared" si="10"/>
-        <v>39.25</v>
+        <v>38.75</v>
       </c>
       <c r="X11">
         <f t="shared" si="11"/>
-        <v>65.416666666666671</v>
+        <v>64.583333333333343</v>
       </c>
       <c r="Y11">
         <f t="shared" si="12"/>
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="Z11" s="20">
         <v>6</v>
@@ -2414,7 +2411,7 @@
       </c>
       <c r="AE11">
         <f t="shared" si="13"/>
-        <v>62.75</v>
+        <v>62.25</v>
       </c>
       <c r="AF11">
         <f t="shared" si="14"/>
@@ -2457,18 +2454,18 @@
         <v>68.75</v>
       </c>
       <c r="K12">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L12">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="M12">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>2.75</v>
       </c>
       <c r="N12">
         <f t="shared" si="5"/>
-        <v>25</v>
+        <v>17.1875</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -2485,30 +2482,30 @@
         <v>0</v>
       </c>
       <c r="S12">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="T12">
         <v>1</v>
       </c>
       <c r="U12">
         <f t="shared" si="8"/>
-        <v>9.75</v>
+        <v>14.75</v>
       </c>
       <c r="V12">
         <f t="shared" si="9"/>
-        <v>60.9375</v>
+        <v>92.1875</v>
       </c>
       <c r="W12">
         <f t="shared" si="10"/>
-        <v>38</v>
+        <v>41.75</v>
       </c>
       <c r="X12">
         <f t="shared" si="11"/>
-        <v>63.333333333333329</v>
+        <v>69.583333333333329</v>
       </c>
       <c r="Y12">
         <f t="shared" si="12"/>
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="Z12" s="20">
         <v>9.5</v>
@@ -2525,11 +2522,11 @@
       </c>
       <c r="AE12">
         <f t="shared" si="13"/>
-        <v>73.5</v>
+        <v>77.25</v>
       </c>
       <c r="AF12">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -2568,18 +2565,18 @@
         <v>81.25</v>
       </c>
       <c r="K13">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L13">
         <v>3</v>
       </c>
       <c r="M13">
         <f t="shared" si="4"/>
-        <v>5.25</v>
+        <v>7.25</v>
       </c>
       <c r="N13">
         <f t="shared" si="5"/>
-        <v>32.8125</v>
+        <v>45.3125</v>
       </c>
       <c r="O13">
         <v>0</v>
@@ -2596,30 +2593,30 @@
         <v>0</v>
       </c>
       <c r="S13">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="T13">
         <v>1</v>
       </c>
       <c r="U13">
         <f t="shared" si="8"/>
-        <v>12.75</v>
+        <v>13.75</v>
       </c>
       <c r="V13">
         <f t="shared" si="9"/>
-        <v>79.6875</v>
+        <v>85.9375</v>
       </c>
       <c r="W13">
         <f t="shared" si="10"/>
-        <v>43.75</v>
+        <v>46.75</v>
       </c>
       <c r="X13">
         <f t="shared" si="11"/>
-        <v>72.916666666666657</v>
+        <v>77.916666666666671</v>
       </c>
       <c r="Y13">
         <f t="shared" si="12"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="Z13" s="19">
         <v>7</v>
@@ -2636,7 +2633,7 @@
       </c>
       <c r="AE13">
         <f t="shared" si="13"/>
-        <v>69.75</v>
+        <v>72.75</v>
       </c>
       <c r="AF13">
         <f t="shared" si="14"/>
@@ -2751,7 +2748,7 @@
       </c>
       <c r="AF14">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -3183,30 +3180,30 @@
         <v>0</v>
       </c>
       <c r="S20">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="T20">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U20">
         <f t="shared" si="8"/>
-        <v>11.25</v>
+        <v>12.5</v>
       </c>
       <c r="V20">
         <f t="shared" si="9"/>
-        <v>70.3125</v>
+        <v>78.125</v>
       </c>
       <c r="W20">
         <f t="shared" si="10"/>
-        <v>42.5</v>
+        <v>43.75</v>
       </c>
       <c r="X20">
         <f t="shared" si="11"/>
-        <v>70.833333333333343</v>
+        <v>72.916666666666657</v>
       </c>
       <c r="Y20">
         <f t="shared" si="12"/>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="Z20" s="20">
         <v>7.5</v>
@@ -3223,11 +3220,11 @@
       </c>
       <c r="AE20">
         <f t="shared" si="13"/>
-        <v>68.5</v>
+        <v>69.75</v>
       </c>
       <c r="AF20">
         <f t="shared" si="14"/>
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21" spans="1:32" ht="15" customHeight="1" thickBot="1">
@@ -3255,15 +3252,15 @@
         <v>8</v>
       </c>
       <c r="H21">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I21">
         <f t="shared" si="2"/>
-        <v>7.25</v>
+        <v>7</v>
       </c>
       <c r="J21">
         <f t="shared" si="3"/>
-        <v>60.416666666666664</v>
+        <v>58.333333333333336</v>
       </c>
       <c r="K21">
         <v>8</v>
@@ -3294,30 +3291,30 @@
         <v>0</v>
       </c>
       <c r="S21">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="T21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U21">
         <f t="shared" si="8"/>
-        <v>11</v>
+        <v>13.75</v>
       </c>
       <c r="V21">
         <f t="shared" si="9"/>
-        <v>68.75</v>
+        <v>85.9375</v>
       </c>
       <c r="W21">
         <f t="shared" si="10"/>
-        <v>38.75</v>
+        <v>41.25</v>
       </c>
       <c r="X21">
         <f t="shared" si="11"/>
-        <v>64.583333333333343</v>
+        <v>68.75</v>
       </c>
       <c r="Y21">
         <f t="shared" si="12"/>
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="Z21" s="19">
         <v>6</v>
@@ -3334,11 +3331,11 @@
       </c>
       <c r="AE21">
         <f t="shared" si="13"/>
-        <v>67.75</v>
+        <v>70.25</v>
       </c>
       <c r="AF21">
         <f t="shared" si="14"/>
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="22" spans="1:32" ht="15" customHeight="1" thickBot="1">
@@ -3428,7 +3425,7 @@
       </c>
       <c r="Y22">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z22" s="20">
         <v>9</v>
@@ -3516,30 +3513,30 @@
         <v>0</v>
       </c>
       <c r="S23">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="T23">
         <v>2</v>
       </c>
       <c r="U23">
         <f t="shared" si="8"/>
-        <v>9.5</v>
+        <v>11.5</v>
       </c>
       <c r="V23">
         <f t="shared" si="9"/>
-        <v>59.375</v>
+        <v>71.875</v>
       </c>
       <c r="W23">
         <f t="shared" si="10"/>
-        <v>40.25</v>
+        <v>42.25</v>
       </c>
       <c r="X23">
         <f t="shared" si="11"/>
-        <v>67.083333333333329</v>
+        <v>70.416666666666671</v>
       </c>
       <c r="Y23">
         <f t="shared" si="12"/>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Z23" s="20">
         <v>7</v>
@@ -3556,7 +3553,7 @@
       </c>
       <c r="AE23">
         <f t="shared" si="13"/>
-        <v>73.25</v>
+        <v>75.25</v>
       </c>
       <c r="AF23">
         <f t="shared" si="14"/>
@@ -3588,29 +3585,29 @@
         <v>10</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I24">
         <f t="shared" si="2"/>
-        <v>9.75</v>
+        <v>9.5</v>
       </c>
       <c r="J24">
         <f t="shared" si="3"/>
-        <v>81.25</v>
+        <v>79.166666666666657</v>
       </c>
       <c r="K24">
         <v>9</v>
       </c>
       <c r="L24">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M24">
         <f t="shared" si="4"/>
-        <v>8.25</v>
+        <v>8</v>
       </c>
       <c r="N24">
         <f t="shared" si="5"/>
-        <v>51.5625</v>
+        <v>50</v>
       </c>
       <c r="O24">
         <v>14</v>
@@ -3642,15 +3639,15 @@
       </c>
       <c r="W24">
         <f t="shared" si="10"/>
-        <v>46.25</v>
+        <v>45.75</v>
       </c>
       <c r="X24">
         <f t="shared" si="11"/>
-        <v>77.083333333333343</v>
+        <v>76.25</v>
       </c>
       <c r="Y24">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="Z24" s="19">
         <v>8.5</v>
@@ -3667,7 +3664,7 @@
       <c r="AD24" s="21"/>
       <c r="AE24">
         <f t="shared" si="13"/>
-        <v>78.25</v>
+        <v>77.75</v>
       </c>
       <c r="AF24">
         <f t="shared" si="14"/>
@@ -3696,32 +3693,32 @@
         <v>100</v>
       </c>
       <c r="G25">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H25">
         <v>3</v>
       </c>
       <c r="I25">
         <f t="shared" si="2"/>
-        <v>7.25</v>
+        <v>8.25</v>
       </c>
       <c r="J25">
         <f t="shared" si="3"/>
-        <v>60.416666666666664</v>
+        <v>68.75</v>
       </c>
       <c r="K25">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M25">
         <f t="shared" si="4"/>
-        <v>8.5</v>
+        <v>9.25</v>
       </c>
       <c r="N25">
         <f t="shared" si="5"/>
-        <v>53.125</v>
+        <v>57.8125</v>
       </c>
       <c r="O25">
         <v>0</v>
@@ -3738,30 +3735,30 @@
         <v>0</v>
       </c>
       <c r="S25">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="T25">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U25">
         <f t="shared" si="8"/>
-        <v>11.5</v>
+        <v>10.25</v>
       </c>
       <c r="V25">
         <f t="shared" si="9"/>
-        <v>71.875</v>
+        <v>64.0625</v>
       </c>
       <c r="W25">
         <f t="shared" si="10"/>
-        <v>43.25</v>
+        <v>43.75</v>
       </c>
       <c r="X25">
         <f t="shared" si="11"/>
-        <v>72.083333333333329</v>
+        <v>72.916666666666657</v>
       </c>
       <c r="Y25">
         <f t="shared" si="12"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Z25" s="20">
         <v>9</v>
@@ -3778,11 +3775,11 @@
       </c>
       <c r="AE25">
         <f t="shared" si="13"/>
-        <v>73.25</v>
+        <v>73.75</v>
       </c>
       <c r="AF25">
         <f t="shared" si="14"/>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="26" spans="1:32" ht="29.4" thickBot="1">
@@ -3852,23 +3849,23 @@
         <v>9</v>
       </c>
       <c r="T26">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="U26">
         <f t="shared" si="8"/>
-        <v>8.5</v>
+        <v>8.25</v>
       </c>
       <c r="V26">
         <f t="shared" si="9"/>
-        <v>53.125</v>
+        <v>51.5625</v>
       </c>
       <c r="W26">
         <f t="shared" si="10"/>
-        <v>35</v>
+        <v>34.75</v>
       </c>
       <c r="X26">
         <f t="shared" si="11"/>
-        <v>58.333333333333336</v>
+        <v>57.916666666666671</v>
       </c>
       <c r="Y26">
         <f t="shared" si="12"/>
@@ -3889,7 +3886,7 @@
       </c>
       <c r="AE26">
         <f t="shared" si="13"/>
-        <v>61.5</v>
+        <v>61.25</v>
       </c>
       <c r="AF26">
         <f t="shared" si="14"/>
@@ -4056,7 +4053,7 @@
         <v>105</v>
       </c>
       <c r="K2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="L2" t="s">
         <v>106</v>
@@ -4080,7 +4077,7 @@
         <v>109</v>
       </c>
       <c r="T2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="V2" t="s">
         <v>110</v>
@@ -4092,13 +4089,13 @@
         <v>111</v>
       </c>
       <c r="Y2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="Z2" t="s">
         <v>112</v>
       </c>
       <c r="AA2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AC2" t="s">
         <v>113</v>
@@ -4110,7 +4107,7 @@
         <v>114</v>
       </c>
       <c r="AF2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="AG2" t="s">
         <v>115</v>
@@ -4151,64 +4148,64 @@
         <v>2</v>
       </c>
       <c r="L3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="M3">
         <v>8</v>
       </c>
       <c r="O3" t="s">
+        <v>120</v>
+      </c>
+      <c r="P3">
+        <v>15</v>
+      </c>
+      <c r="Q3" t="s">
         <v>121</v>
       </c>
-      <c r="P3">
-        <v>14</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="R3">
+        <v>9</v>
+      </c>
+      <c r="S3" t="s">
         <v>122</v>
-      </c>
-      <c r="R3">
-        <v>10</v>
-      </c>
-      <c r="S3" t="s">
-        <v>123</v>
       </c>
       <c r="T3">
         <v>9</v>
       </c>
       <c r="V3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="W3">
         <v>4</v>
       </c>
       <c r="X3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="Y3">
         <v>16</v>
       </c>
       <c r="Z3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="AA3">
         <v>3</v>
       </c>
       <c r="AC3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="AD3">
         <v>16</v>
       </c>
       <c r="AE3" t="s">
+        <v>127</v>
+      </c>
+      <c r="AF3">
+        <v>7</v>
+      </c>
+      <c r="AG3" t="s">
         <v>128</v>
       </c>
-      <c r="AF3">
-        <v>9</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>114</v>
-      </c>
       <c r="AH3">
-        <v>5</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:34">
@@ -4237,28 +4234,28 @@
         <v>17</v>
       </c>
       <c r="J4" t="s">
-        <v>120</v>
+        <v>133</v>
       </c>
       <c r="K4">
         <v>2</v>
       </c>
       <c r="L4" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="M4">
         <v>6</v>
       </c>
       <c r="O4" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="P4">
         <v>13</v>
       </c>
       <c r="Q4" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="R4">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="S4" t="s">
         <v>135</v>
@@ -4276,7 +4273,7 @@
         <v>137</v>
       </c>
       <c r="Y4">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Z4" t="s">
         <v>138</v>
@@ -4291,13 +4288,13 @@
         <v>16</v>
       </c>
       <c r="AE4" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="AF4">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="AG4" t="s">
-        <v>140</v>
+        <v>114</v>
       </c>
       <c r="AH4">
         <v>4</v>
@@ -4305,91 +4302,91 @@
     </row>
     <row r="5" spans="1:34">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B5">
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="F5">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="I5">
         <v>17</v>
       </c>
       <c r="J5" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K5">
         <v>1</v>
       </c>
       <c r="L5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="M5">
         <v>4</v>
       </c>
       <c r="O5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="P5">
         <v>12</v>
       </c>
       <c r="Q5" t="s">
+        <v>147</v>
+      </c>
+      <c r="R5">
+        <v>7</v>
+      </c>
+      <c r="S5" t="s">
         <v>148</v>
-      </c>
-      <c r="R5">
-        <v>8</v>
-      </c>
-      <c r="S5" t="s">
-        <v>149</v>
       </c>
       <c r="T5">
         <v>7</v>
       </c>
       <c r="V5" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="W5">
         <v>3</v>
       </c>
       <c r="X5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="Y5">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="Z5" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="AA5">
         <v>3</v>
       </c>
       <c r="AC5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="AD5">
         <v>16</v>
       </c>
       <c r="AE5" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="AF5">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="AG5" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="AH5">
         <v>3</v>
@@ -4397,7 +4394,7 @@
     </row>
     <row r="6" spans="1:34">
       <c r="A6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B6">
         <v>18</v>
@@ -4409,55 +4406,55 @@
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F6">
         <v>1</v>
       </c>
       <c r="H6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="I6">
         <v>17</v>
       </c>
       <c r="J6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="K6">
         <v>1</v>
       </c>
       <c r="L6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M6">
         <v>3</v>
       </c>
       <c r="O6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="P6">
         <v>11</v>
       </c>
       <c r="Q6" t="s">
-        <v>123</v>
+        <v>158</v>
       </c>
       <c r="R6">
+        <v>6</v>
+      </c>
+      <c r="S6" t="s">
+        <v>147</v>
+      </c>
+      <c r="T6">
         <v>7</v>
       </c>
-      <c r="S6" t="s">
-        <v>148</v>
-      </c>
-      <c r="T6">
-        <v>6</v>
-      </c>
       <c r="V6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="W6">
         <v>3</v>
       </c>
       <c r="X6" t="s">
-        <v>150</v>
+        <v>160</v>
       </c>
       <c r="Y6">
         <v>15</v>
@@ -4472,19 +4469,19 @@
         <v>162</v>
       </c>
       <c r="AD6">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AE6" t="s">
         <v>163</v>
       </c>
       <c r="AF6">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="AG6" t="s">
         <v>164</v>
       </c>
       <c r="AH6">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:34">
@@ -4507,7 +4504,7 @@
         <v>1</v>
       </c>
       <c r="H7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="I7">
         <v>17</v>
@@ -4519,69 +4516,69 @@
         <v>0</v>
       </c>
       <c r="L7" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="M7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="O7" t="s">
+        <v>158</v>
+      </c>
+      <c r="P7">
+        <v>9</v>
+      </c>
+      <c r="Q7" t="s">
         <v>167</v>
-      </c>
-      <c r="P7">
-        <v>8</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>168</v>
       </c>
       <c r="R7">
         <v>6</v>
       </c>
       <c r="S7" t="s">
-        <v>159</v>
+        <v>167</v>
       </c>
       <c r="T7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="V7" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="W7">
         <v>2</v>
       </c>
       <c r="X7" t="s">
+        <v>125</v>
+      </c>
+      <c r="Y7">
+        <v>14</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>168</v>
+      </c>
+      <c r="AA7">
+        <v>3</v>
+      </c>
+      <c r="AC7" t="s">
         <v>169</v>
-      </c>
-      <c r="Y7">
-        <v>15</v>
-      </c>
-      <c r="Z7" t="s">
-        <v>170</v>
-      </c>
-      <c r="AA7">
-        <v>2</v>
-      </c>
-      <c r="AC7" t="s">
-        <v>171</v>
       </c>
       <c r="AD7">
         <v>15</v>
       </c>
       <c r="AE7" t="s">
-        <v>172</v>
+        <v>153</v>
       </c>
       <c r="AF7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AG7" t="s">
-        <v>162</v>
+        <v>127</v>
       </c>
       <c r="AH7">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:34">
       <c r="A8" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="B8">
         <v>18</v>
@@ -4599,7 +4596,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="I8">
         <v>14</v>
@@ -4611,61 +4608,61 @@
         <v>0</v>
       </c>
       <c r="L8" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="M8">
         <v>1</v>
       </c>
       <c r="O8" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="P8">
         <v>8</v>
       </c>
       <c r="Q8" t="s">
-        <v>149</v>
+        <v>171</v>
       </c>
       <c r="R8">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="S8" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="T8">
         <v>5</v>
       </c>
       <c r="V8" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="W8">
         <v>2</v>
       </c>
       <c r="X8" t="s">
-        <v>170</v>
+        <v>138</v>
       </c>
       <c r="Y8">
+        <v>14</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>172</v>
+      </c>
+      <c r="AA8">
+        <v>3</v>
+      </c>
+      <c r="AC8" t="s">
+        <v>173</v>
+      </c>
+      <c r="AD8">
         <v>15</v>
       </c>
-      <c r="Z8" t="s">
-        <v>169</v>
-      </c>
-      <c r="AA8">
-        <v>1</v>
-      </c>
-      <c r="AC8" t="s">
-        <v>164</v>
-      </c>
-      <c r="AD8">
-        <v>14</v>
-      </c>
       <c r="AE8" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="AF8">
         <v>3</v>
       </c>
       <c r="AG8" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="AH8">
         <v>1</v>
@@ -4673,7 +4670,7 @@
     </row>
     <row r="9" spans="1:34">
       <c r="A9" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B9">
         <v>18</v>
@@ -4691,49 +4688,49 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="I9">
         <v>14</v>
       </c>
       <c r="J9" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K9">
         <v>0</v>
       </c>
       <c r="L9" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="M9">
         <v>1</v>
       </c>
       <c r="O9" t="s">
-        <v>168</v>
+        <v>176</v>
       </c>
       <c r="P9">
         <v>8</v>
       </c>
       <c r="Q9" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
       <c r="R9">
         <v>5</v>
       </c>
       <c r="S9" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="T9">
         <v>5</v>
       </c>
       <c r="V9" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="W9">
         <v>1</v>
       </c>
       <c r="X9" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="Y9">
         <v>14</v>
@@ -4742,22 +4739,22 @@
         <v>160</v>
       </c>
       <c r="AA9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AC9" t="s">
-        <v>175</v>
+        <v>163</v>
       </c>
       <c r="AD9">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AE9" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
       <c r="AF9">
         <v>3</v>
       </c>
       <c r="AG9" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="AH9">
         <v>1</v>
@@ -4783,73 +4780,73 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="I10">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="J10" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="K10">
         <v>0</v>
       </c>
       <c r="L10" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
       <c r="M10">
         <v>1</v>
       </c>
       <c r="O10" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="P10">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Q10" t="s">
-        <v>174</v>
+        <v>109</v>
       </c>
       <c r="R10">
+        <v>4</v>
+      </c>
+      <c r="S10" t="s">
+        <v>176</v>
+      </c>
+      <c r="T10">
         <v>5</v>
       </c>
-      <c r="S10" t="s">
-        <v>147</v>
-      </c>
-      <c r="T10">
-        <v>4</v>
-      </c>
       <c r="V10" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="W10">
         <v>1</v>
       </c>
       <c r="X10" t="s">
-        <v>126</v>
+        <v>150</v>
       </c>
       <c r="Y10">
         <v>14</v>
       </c>
       <c r="Z10" t="s">
-        <v>137</v>
+        <v>149</v>
       </c>
       <c r="AA10">
         <v>1</v>
       </c>
       <c r="AC10" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="AD10">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="AE10" t="s">
-        <v>155</v>
+        <v>113</v>
       </c>
       <c r="AF10">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG10" t="s">
-        <v>128</v>
+        <v>174</v>
       </c>
       <c r="AH10">
         <v>1</v>
@@ -4863,7 +4860,7 @@
         <v>17</v>
       </c>
       <c r="C11" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -4875,7 +4872,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>119</v>
+        <v>105</v>
       </c>
       <c r="I11">
         <v>10</v>
@@ -4887,64 +4884,64 @@
         <v>0</v>
       </c>
       <c r="L11" t="s">
-        <v>104</v>
+        <v>155</v>
       </c>
       <c r="M11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O11" t="s">
-        <v>135</v>
+        <v>108</v>
       </c>
       <c r="P11">
         <v>6</v>
       </c>
       <c r="Q11" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="R11">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="S11" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="T11">
         <v>4</v>
       </c>
       <c r="V11" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="W11">
         <v>1</v>
       </c>
       <c r="X11" t="s">
-        <v>110</v>
+        <v>161</v>
       </c>
       <c r="Y11">
         <v>14</v>
       </c>
       <c r="Z11" t="s">
-        <v>111</v>
+        <v>159</v>
       </c>
       <c r="AA11">
         <v>1</v>
       </c>
       <c r="AC11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="AD11">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="AE11" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="AF11">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AG11" t="s">
-        <v>163</v>
+        <v>113</v>
       </c>
       <c r="AH11">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -4973,11 +4970,11 @@
     <col min="19" max="21" width="8" customWidth="1"/>
     <col min="22" max="30" width="7" customWidth="1"/>
     <col min="31" max="31" width="8" customWidth="1"/>
-    <col min="32" max="33" width="7" customWidth="1"/>
-    <col min="34" max="34" width="8" customWidth="1"/>
-    <col min="35" max="74" width="7" customWidth="1"/>
-    <col min="75" max="75" width="8" customWidth="1"/>
-    <col min="76" max="78" width="7" customWidth="1"/>
+    <col min="32" max="32" width="7" customWidth="1"/>
+    <col min="33" max="34" width="8" customWidth="1"/>
+    <col min="35" max="35" width="7" customWidth="1"/>
+    <col min="36" max="37" width="8" customWidth="1"/>
+    <col min="38" max="78" width="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:78">
@@ -4991,28 +4988,28 @@
         <v>101</v>
       </c>
       <c r="D1" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E1" s="14" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F1" s="14" t="s">
         <v>165</v>
       </c>
       <c r="G1" s="14" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="H1" s="14" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J1" s="14" t="s">
         <v>166</v>
       </c>
       <c r="K1" s="14" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="L1" s="14" t="s">
         <v>131</v>
@@ -5039,46 +5036,46 @@
         <v>118</v>
       </c>
       <c r="T1" s="14" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="U1" s="14" t="s">
         <v>132</v>
       </c>
       <c r="V1" s="14" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="W1" s="14" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="X1" s="14" t="s">
         <v>104</v>
       </c>
       <c r="Y1" s="14" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="Z1" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA1" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="AA1" s="14" t="s">
-        <v>120</v>
-      </c>
       <c r="AB1" s="14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AC1" s="14" t="s">
         <v>106</v>
       </c>
       <c r="AD1" s="14" t="s">
-        <v>105</v>
+        <v>133</v>
       </c>
       <c r="AE1" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="AF1" s="14" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="AG1" s="14" t="s">
-        <v>167</v>
+        <v>171</v>
       </c>
       <c r="AH1" s="14" t="s">
         <v>109</v>
@@ -5087,7 +5084,7 @@
         <v>108</v>
       </c>
       <c r="AJ1" s="14" t="s">
-        <v>121</v>
+        <v>134</v>
       </c>
       <c r="AK1" s="14" t="s">
         <v>135</v>
@@ -5096,124 +5093,124 @@
         <v>107</v>
       </c>
       <c r="AM1" s="14" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="AN1" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="AO1" s="14" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="AP1" s="14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="AQ1" s="14" t="s">
-        <v>133</v>
+        <v>120</v>
       </c>
       <c r="AR1" s="14" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="AS1" s="14" t="s">
-        <v>134</v>
+        <v>167</v>
       </c>
       <c r="AT1" s="14" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="AU1" s="14" t="s">
-        <v>112</v>
+        <v>125</v>
       </c>
       <c r="AV1" s="14" t="s">
-        <v>150</v>
+        <v>137</v>
       </c>
       <c r="AW1" s="14" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="AX1" s="14" t="s">
         <v>110</v>
       </c>
       <c r="AY1" s="14" t="s">
-        <v>138</v>
+        <v>150</v>
       </c>
       <c r="AZ1" s="14" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="BA1" s="14" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
       <c r="BB1" s="14" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="BC1" s="14" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="BD1" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="BE1" s="14" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="BF1" s="14" t="s">
         <v>136</v>
       </c>
       <c r="BG1" s="14" t="s">
-        <v>137</v>
+        <v>172</v>
       </c>
       <c r="BH1" s="14" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="BI1" s="14" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="BJ1" s="14" t="s">
-        <v>151</v>
+        <v>124</v>
       </c>
       <c r="BK1" s="14" t="s">
         <v>113</v>
       </c>
       <c r="BL1" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="BM1" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="BN1" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="BO1" s="14" t="s">
+        <v>163</v>
+      </c>
+      <c r="BP1" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="BQ1" s="14" t="s">
+        <v>153</v>
+      </c>
+      <c r="BR1" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="BS1" s="14" t="s">
         <v>164</v>
-      </c>
-      <c r="BM1" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="BN1" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="BO1" s="14" t="s">
-        <v>171</v>
-      </c>
-      <c r="BP1" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="BQ1" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="BR1" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="BS1" s="14" t="s">
-        <v>172</v>
       </c>
       <c r="BT1" s="14" t="s">
         <v>139</v>
       </c>
       <c r="BU1" s="14" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="BV1" s="14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="BW1" s="14" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="BX1" s="14" t="s">
         <v>115</v>
       </c>
       <c r="BY1" s="14" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="BZ1" s="14" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
     </row>
     <row r="2" spans="1:78">
@@ -5304,7 +5301,9 @@
       <c r="AC2" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="AD2" s="18"/>
+      <c r="AD2" s="16" t="s">
+        <v>180</v>
+      </c>
       <c r="AE2" s="18"/>
       <c r="AF2" s="18"/>
       <c r="AG2" s="18"/>
@@ -5363,7 +5362,9 @@
       <c r="BH2" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="BI2" s="18"/>
+      <c r="BI2" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="BJ2" s="17" t="s">
         <v>183</v>
       </c>
@@ -5409,7 +5410,9 @@
       <c r="BX2" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="BY2" s="18"/>
+      <c r="BY2" s="16" t="s">
+        <v>178</v>
+      </c>
       <c r="BZ2" s="16" t="s">
         <v>180</v>
       </c>
@@ -5502,7 +5505,9 @@
       <c r="AC3" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="AD3" s="18"/>
+      <c r="AD3" s="16" t="s">
+        <v>180</v>
+      </c>
       <c r="AE3" s="16" t="s">
         <v>178</v>
       </c>
@@ -5596,7 +5601,9 @@
       <c r="BU3" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="BV3" s="18"/>
+      <c r="BV3" s="16" t="s">
+        <v>178</v>
+      </c>
       <c r="BW3" s="16" t="s">
         <v>180</v>
       </c>
@@ -5735,7 +5742,9 @@
       <c r="AP4" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="AQ4" s="18"/>
+      <c r="AQ4" s="16" t="s">
+        <v>180</v>
+      </c>
       <c r="AR4" s="17" t="s">
         <v>182</v>
       </c>
@@ -6325,11 +6334,15 @@
       <c r="BF8" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="BG8" s="18"/>
+      <c r="BG8" s="17" t="s">
+        <v>182</v>
+      </c>
       <c r="BH8" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="BI8" s="18"/>
+      <c r="BI8" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="BJ8" s="18"/>
       <c r="BK8" s="16" t="s">
         <v>178</v>
@@ -6373,7 +6386,9 @@
       <c r="BX8" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="BY8" s="18"/>
+      <c r="BY8" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="BZ8" s="16" t="s">
         <v>180</v>
       </c>
@@ -6494,8 +6509,12 @@
       <c r="AO9" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="AP9" s="18"/>
-      <c r="AQ9" s="18"/>
+      <c r="AP9" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="AQ9" s="16" t="s">
+        <v>180</v>
+      </c>
       <c r="AR9" s="16" t="s">
         <v>180</v>
       </c>
@@ -6535,9 +6554,13 @@
       <c r="BF9" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="BG9" s="18"/>
+      <c r="BG9" s="17" t="s">
+        <v>182</v>
+      </c>
       <c r="BH9" s="18"/>
-      <c r="BI9" s="18"/>
+      <c r="BI9" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="BJ9" s="18"/>
       <c r="BK9" s="18"/>
       <c r="BL9" s="18"/>
@@ -6697,7 +6720,9 @@
       <c r="AR11" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="AS11" s="18"/>
+      <c r="AS11" s="17" t="s">
+        <v>184</v>
+      </c>
       <c r="AT11" s="17" t="s">
         <v>182</v>
       </c>
@@ -6759,7 +6784,9 @@
       <c r="BX11" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="BY11" s="18"/>
+      <c r="BY11" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="BZ11" s="16" t="s">
         <v>180</v>
       </c>
@@ -6862,17 +6889,17 @@
         <v>182</v>
       </c>
       <c r="AG12" s="17" t="s">
-        <v>185</v>
-      </c>
-      <c r="AH12" s="16" t="s">
-        <v>178</v>
+        <v>186</v>
+      </c>
+      <c r="AH12" s="17" t="s">
+        <v>186</v>
       </c>
       <c r="AI12" s="18"/>
-      <c r="AJ12" s="16" t="s">
-        <v>180</v>
+      <c r="AJ12" s="17" t="s">
+        <v>187</v>
       </c>
       <c r="AK12" s="17" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="AL12" s="16" t="s">
         <v>179</v>
@@ -6881,8 +6908,8 @@
         <v>180</v>
       </c>
       <c r="AN12" s="18"/>
-      <c r="AO12" s="17" t="s">
-        <v>184</v>
+      <c r="AO12" s="16" t="s">
+        <v>180</v>
       </c>
       <c r="AP12" s="17" t="s">
         <v>183</v>
@@ -6918,7 +6945,9 @@
       <c r="BK12" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="BL12" s="18"/>
+      <c r="BL12" s="16" t="s">
+        <v>181</v>
+      </c>
       <c r="BM12" s="16" t="s">
         <v>178</v>
       </c>
@@ -6943,13 +6972,21 @@
       <c r="BT12" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="BU12" s="18"/>
-      <c r="BV12" s="18"/>
-      <c r="BW12" s="18"/>
+      <c r="BU12" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="BV12" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="BW12" s="16" t="s">
+        <v>180</v>
+      </c>
       <c r="BX12" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="BY12" s="18"/>
+      <c r="BY12" s="16" t="s">
+        <v>178</v>
+      </c>
       <c r="BZ12" s="16" t="s">
         <v>180</v>
       </c>
@@ -7074,8 +7111,12 @@
       <c r="AQ13" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="AR13" s="18"/>
-      <c r="AS13" s="18"/>
+      <c r="AR13" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="AS13" s="16" t="s">
+        <v>179</v>
+      </c>
       <c r="AT13" s="18"/>
       <c r="AU13" s="18"/>
       <c r="AV13" s="18"/>
@@ -7133,7 +7174,9 @@
       <c r="BX13" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="BY13" s="18"/>
+      <c r="BY13" s="16" t="s">
+        <v>178</v>
+      </c>
       <c r="BZ13" s="16" t="s">
         <v>180</v>
       </c>
@@ -7557,8 +7600,8 @@
       <c r="BV20" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="BW20" s="17" t="s">
-        <v>189</v>
+      <c r="BW20" s="16" t="s">
+        <v>180</v>
       </c>
       <c r="BX20" s="16" t="s">
         <v>179</v>
@@ -7656,7 +7699,9 @@
       <c r="AC21" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="AD21" s="18"/>
+      <c r="AD21" s="17" t="s">
+        <v>184</v>
+      </c>
       <c r="AE21" s="16" t="s">
         <v>178</v>
       </c>
@@ -7745,11 +7790,19 @@
       <c r="BT21" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="BU21" s="18"/>
+      <c r="BU21" s="17" t="s">
+        <v>182</v>
+      </c>
       <c r="BV21" s="18"/>
-      <c r="BW21" s="18"/>
-      <c r="BX21" s="18"/>
-      <c r="BY21" s="18"/>
+      <c r="BW21" s="16" t="s">
+        <v>180</v>
+      </c>
+      <c r="BX21" s="16" t="s">
+        <v>179</v>
+      </c>
+      <c r="BY21" s="16" t="s">
+        <v>178</v>
+      </c>
       <c r="BZ21" s="16" t="s">
         <v>180</v>
       </c>
@@ -8128,8 +8181,12 @@
       <c r="BU23" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="BV23" s="18"/>
-      <c r="BW23" s="18"/>
+      <c r="BV23" s="16" t="s">
+        <v>178</v>
+      </c>
+      <c r="BW23" s="16" t="s">
+        <v>180</v>
+      </c>
       <c r="BX23" s="17" t="s">
         <v>184</v>
       </c>
@@ -8226,7 +8283,9 @@
       <c r="AC24" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="AD24" s="18"/>
+      <c r="AD24" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="AE24" s="17" t="s">
         <v>183</v>
       </c>
@@ -8265,7 +8324,9 @@
       <c r="AR24" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="AS24" s="18"/>
+      <c r="AS24" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="AT24" s="18"/>
       <c r="AU24" s="16" t="s">
         <v>180</v>
@@ -8420,7 +8481,9 @@
       <c r="AC25" s="17" t="s">
         <v>182</v>
       </c>
-      <c r="AD25" s="18"/>
+      <c r="AD25" s="16" t="s">
+        <v>180</v>
+      </c>
       <c r="AE25" s="16" t="s">
         <v>178</v>
       </c>
@@ -8454,11 +8517,15 @@
       <c r="AQ25" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="AR25" s="18"/>
+      <c r="AR25" s="16" t="s">
+        <v>180</v>
+      </c>
       <c r="AS25" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="AT25" s="18"/>
+      <c r="AT25" s="17" t="s">
+        <v>183</v>
+      </c>
       <c r="AU25" s="18"/>
       <c r="AV25" s="18"/>
       <c r="AW25" s="18"/>
@@ -8499,7 +8566,9 @@
       <c r="BR25" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="BS25" s="18"/>
+      <c r="BS25" s="17" t="s">
+        <v>185</v>
+      </c>
       <c r="BT25" s="16" t="s">
         <v>178</v>
       </c>
@@ -8513,9 +8582,7 @@
       <c r="BX25" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="BY25" s="16" t="s">
-        <v>178</v>
-      </c>
+      <c r="BY25" s="18"/>
       <c r="BZ25" s="16" t="s">
         <v>180</v>
       </c>
@@ -8689,7 +8756,9 @@
       <c r="BX26" s="17" t="s">
         <v>184</v>
       </c>
-      <c r="BY26" s="18"/>
+      <c r="BY26" s="17" t="s">
+        <v>182</v>
+      </c>
       <c r="BZ26" s="16" t="s">
         <v>180</v>
       </c>

</xml_diff>

<commit_message>
Update test results data - 2025-04-12 01:36 PM
Generated with VH Results Processing System

Processing completed:

- Processed IBA tests (Simple and Full)

- Processed FBS mock tests

- Generated optimized JSON files for Vercel deployment

- Updated students database

- Synced student emails from MongoDB

- Synced roleNumbers to MongoDB for FBS access
</commit_message>
<xml_diff>
--- a/Results/DU FBS Mocks/DU FBS Mock 5.xlsx
+++ b/Results/DU FBS Mocks/DU FBS Mock 5.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\results giver\FBS Result Giver\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VH Website\vh-website\Results\DU FBS Mocks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE50521-A704-44D1-BC2E-2B3DC79D9D91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD38EB6E-D74B-4110-AEFB-E71A0B0D979F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1251,8 +1251,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AI27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="80" workbookViewId="0">
-      <selection activeCell="AE14" sqref="AE14"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="80" workbookViewId="0">
+      <selection activeCell="AF12" sqref="AF12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1448,7 +1448,7 @@
       </c>
       <c r="Y2">
         <f t="shared" ref="Y2:Y26" si="12">_xlfn.RANK.EQ(X2, $X$2:$X$1002, 0)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Z2" s="19">
         <v>3</v>
@@ -1563,7 +1563,7 @@
       </c>
       <c r="Y3">
         <f t="shared" si="12"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="Z3" s="20">
         <v>7</v>
@@ -1678,7 +1678,7 @@
       </c>
       <c r="Y4">
         <f t="shared" si="12"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="Z4" s="22">
         <v>3</v>
@@ -1793,7 +1793,7 @@
       </c>
       <c r="Y5">
         <f t="shared" si="12"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Z5" s="20">
         <v>5.5</v>
@@ -1857,18 +1857,18 @@
         <v>70.833333333333343</v>
       </c>
       <c r="K6">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="L6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M6">
         <f t="shared" si="4"/>
-        <v>5</v>
+        <v>6.25</v>
       </c>
       <c r="N6">
         <f t="shared" si="5"/>
-        <v>31.25</v>
+        <v>39.0625</v>
       </c>
       <c r="O6">
         <v>0</v>
@@ -1900,15 +1900,15 @@
       </c>
       <c r="W6">
         <f t="shared" si="10"/>
-        <v>40</v>
+        <v>41.25</v>
       </c>
       <c r="X6">
         <f t="shared" si="11"/>
-        <v>66.666666666666657</v>
+        <v>68.75</v>
       </c>
       <c r="Y6">
         <f t="shared" si="12"/>
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="Z6" s="20">
         <v>6.5</v>
@@ -1925,7 +1925,7 @@
       </c>
       <c r="AE6">
         <f t="shared" si="13"/>
-        <v>65.5</v>
+        <v>66.75</v>
       </c>
       <c r="AF6">
         <f t="shared" si="14"/>
@@ -2145,18 +2145,18 @@
         <v>70.3125</v>
       </c>
       <c r="G9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H9">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I9">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7.25</v>
       </c>
       <c r="J9">
         <f t="shared" si="3"/>
-        <v>50</v>
+        <v>60.416666666666664</v>
       </c>
       <c r="K9">
         <v>10</v>
@@ -2202,11 +2202,11 @@
       </c>
       <c r="W9">
         <f t="shared" si="10"/>
-        <v>28.5</v>
+        <v>29.75</v>
       </c>
       <c r="X9">
         <f t="shared" si="11"/>
-        <v>47.5</v>
+        <v>49.583333333333336</v>
       </c>
       <c r="Y9">
         <f t="shared" si="12"/>
@@ -2227,7 +2227,7 @@
       <c r="AD9" s="21"/>
       <c r="AE9">
         <f t="shared" si="13"/>
-        <v>42.5</v>
+        <v>43.75</v>
       </c>
       <c r="AF9">
         <f t="shared" si="14"/>
@@ -2440,32 +2440,32 @@
         <v>100</v>
       </c>
       <c r="G12">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="H12">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I12">
         <f t="shared" si="2"/>
-        <v>8.25</v>
+        <v>10.75</v>
       </c>
       <c r="J12">
         <f t="shared" si="3"/>
-        <v>68.75</v>
+        <v>89.583333333333343</v>
       </c>
       <c r="K12">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L12">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="M12">
         <f t="shared" si="4"/>
-        <v>2.75</v>
+        <v>5.25</v>
       </c>
       <c r="N12">
         <f t="shared" si="5"/>
-        <v>17.1875</v>
+        <v>32.8125</v>
       </c>
       <c r="O12">
         <v>0</v>
@@ -2497,15 +2497,15 @@
       </c>
       <c r="W12">
         <f t="shared" si="10"/>
-        <v>41.75</v>
+        <v>46.75</v>
       </c>
       <c r="X12">
         <f t="shared" si="11"/>
-        <v>69.583333333333329</v>
+        <v>77.916666666666671</v>
       </c>
       <c r="Y12">
         <f t="shared" si="12"/>
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="Z12" s="20">
         <v>9.5</v>
@@ -2522,11 +2522,11 @@
       </c>
       <c r="AE12">
         <f t="shared" si="13"/>
-        <v>77.25</v>
+        <v>82.25</v>
       </c>
       <c r="AF12">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:35" ht="15" customHeight="1" thickBot="1">
@@ -2616,7 +2616,7 @@
       </c>
       <c r="Y13">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z13" s="19">
         <v>7</v>
@@ -2727,7 +2727,7 @@
       </c>
       <c r="Y14">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Z14" s="20">
         <v>6.5</v>
@@ -3203,7 +3203,7 @@
       </c>
       <c r="Y20">
         <f t="shared" si="12"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Z20" s="20">
         <v>7.5</v>
@@ -3425,7 +3425,7 @@
       </c>
       <c r="Y22">
         <f t="shared" si="12"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Z22" s="20">
         <v>9</v>
@@ -3446,7 +3446,7 @@
       </c>
       <c r="AF22">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="23" spans="1:32" ht="15" customHeight="1" thickBot="1">
@@ -3536,7 +3536,7 @@
       </c>
       <c r="Y23">
         <f t="shared" si="12"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Z23" s="20">
         <v>7</v>
@@ -3568,18 +3568,18 @@
         <v>78</v>
       </c>
       <c r="C24">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E24">
         <f t="shared" si="0"/>
-        <v>14.75</v>
+        <v>16</v>
       </c>
       <c r="F24">
         <f t="shared" si="1"/>
-        <v>92.1875</v>
+        <v>100</v>
       </c>
       <c r="G24">
         <v>10</v>
@@ -3639,15 +3639,15 @@
       </c>
       <c r="W24">
         <f t="shared" si="10"/>
-        <v>45.75</v>
+        <v>47</v>
       </c>
       <c r="X24">
         <f t="shared" si="11"/>
-        <v>76.25</v>
+        <v>78.333333333333329</v>
       </c>
       <c r="Y24">
         <f t="shared" si="12"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="Z24" s="19">
         <v>8.5</v>
@@ -3664,11 +3664,11 @@
       <c r="AD24" s="21"/>
       <c r="AE24">
         <f t="shared" si="13"/>
-        <v>77.75</v>
+        <v>79</v>
       </c>
       <c r="AF24">
         <f t="shared" si="14"/>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:32" ht="43.8" thickBot="1">
@@ -3758,7 +3758,7 @@
       </c>
       <c r="Y25">
         <f t="shared" si="12"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Z25" s="20">
         <v>9</v>

</xml_diff>